<commit_message>
have to finish up excel file, but lgtm! xD
</commit_message>
<xml_diff>
--- a/documentation/SFT221 Workshop 4 Template(1).xlsx
+++ b/documentation/SFT221 Workshop 4 Template(1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://seneca-my.sharepoint.com/personal/ziad_diab_senecapolytechnic_ca/Documents/2247/SFT221/Workshops/ws04/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\School\Fall 2024\SFT221\ws4\Workshop-4\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D3A282F8-8468-4086-84AB-40F65B86D7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8074D2B-46D1-48A5-BCB6-FF3789A2865D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DC3EFA-505A-4B94-B0F7-E545C1BBB447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25320" yWindow="-3360" windowWidth="21000" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Declaration" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Workshop 4</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>SFT221</t>
+  </si>
+  <si>
+    <t>Nicholas Chiong</t>
   </si>
 </sst>
 </file>
@@ -632,7 +635,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="B6" sqref="B6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +670,9 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="14" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -680,7 +685,9 @@
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="16">
+        <v>173163239</v>
+      </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -1625,6 +1632,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="7db3b190-d1cf-4882-bee6-3064ce691739" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100068B9DB3898E1840A1985BE38A336A09" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53950f09b7ed080fb33c20b03183057b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b" xmlns:ns3="7db3b190-d1cf-4882-bee6-3064ce691739" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11827f9efe383da07ec5a4768c75141e" ns2:_="" ns3:_="">
     <xsd:import namespace="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
@@ -1867,27 +1894,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="7db3b190-d1cf-4882-bee6-3064ce691739" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EE4930E-E9D7-44A5-8A50-2884EB163627}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D276BCBD-4FB1-4207-B914-4FC3C0518173}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
+    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CB2FF0-186E-4A4E-B62F-3C149A239155}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1904,23 +1930,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D276BCBD-4FB1-4207-B914-4FC3C0518173}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
-    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EE4930E-E9D7-44A5-8A50-2884EB163627}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>